<commit_message>
implement most features for caxlsx
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -14,22 +14,262 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="27">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="1"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="1"/>
+      <u val="single"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="1"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="1"/>
+      <u val="none"/>
+      <i val="1"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="single"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="20"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="0"/>
+      <u val="none"/>
+      <i val="0"/>
+      <strike val="0"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border/>
     <border>
       <left style="thin">
@@ -44,15 +284,94 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border/>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="29">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="2" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="2" numFmtId="0" fontId="3" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="4" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="5" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="6" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="7" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="8" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="9" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="10" fillId="2" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="3" numFmtId="0" fontId="11" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="4" numFmtId="0" fontId="12" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="5" numFmtId="0" fontId="13" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="6" numFmtId="0" fontId="14" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="7" numFmtId="0" fontId="15" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="8" numFmtId="0" fontId="16" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="17" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="0" fontId="18" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment/>
+    </xf>
+    <xf borderId="0" numFmtId="5" fontId="19" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="14" fontId="20" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="22" fontId="21" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="1" fontId="22" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="9" fontId="23" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="49" fontId="24" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="21" fontId="25" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="48" fontId="26" fillId="0" applyNumberFormat="1" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -73,310 +392,310 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="35.2"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="24.200000000000003"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="24.200000000000003"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="11.0"/>
-    <col min="5" max="5" bestFit="1" customWidth="1" width="11.0"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="44.8"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="30.799999999999997"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="30.799999999999997"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="21.0"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="21.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Header1</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Header2</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Header3</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Header4</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Header5</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="str">
+      <c r="A2" s="7" t="str">
         <f>ADD(1, 2)</f>
       </c>
-      <c r="B2" s="0" t="str">
+      <c r="B2" s="8" t="str">
         <f>1</f>
       </c>
-      <c r="C2" s="0" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>These are variables</t>
         </is>
       </c>
-      <c r="D2" s="0"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>A note</t>
         </is>
       </c>
-      <c r="B3" s="0"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>The font is red</t>
         </is>
       </c>
-      <c r="B4" s="0"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>The font is 'Comic Sans MS'</t>
         </is>
       </c>
-      <c r="B5" s="0"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>The font is size 20</t>
         </is>
       </c>
-      <c r="B6" s="0"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="inlineStr">
+      <c r="A7" s="12" t="inlineStr">
         <is>
           <t>The cell is green</t>
         </is>
       </c>
-      <c r="B7" s="0"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="inlineStr">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>This line is repeated 3 times</t>
         </is>
       </c>
-      <c r="B8" s="0"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="inlineStr">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>This line is repeated 3 times</t>
         </is>
       </c>
-      <c r="B9" s="0"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="inlineStr">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>This line is repeated 3 times</t>
         </is>
       </c>
-      <c r="B10" s="0"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="inlineStr">
+      <c r="A11" s="13" t="inlineStr">
         <is>
           <t>All borders</t>
         </is>
       </c>
-      <c r="B11" s="0"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0" t="inlineStr">
+      <c r="A12" s="9"/>
+      <c r="B12" s="14" t="inlineStr">
         <is>
           <t>Top border</t>
         </is>
       </c>
-      <c r="C12" s="0"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="0" t="inlineStr">
+      <c r="A13" s="15" t="inlineStr">
         <is>
           <t>Bottom border</t>
         </is>
       </c>
-      <c r="B13" s="0"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0" t="inlineStr">
+      <c r="A14" s="9"/>
+      <c r="B14" s="16" t="inlineStr">
         <is>
           <t>Left border</t>
         </is>
       </c>
-      <c r="C14" s="0"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="0" t="inlineStr">
+      <c r="A15" s="17" t="inlineStr">
         <is>
           <t>Right border</t>
         </is>
       </c>
-      <c r="B15" s="0"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0" t="inlineStr">
+      <c r="A16" s="9"/>
+      <c r="B16" s="18" t="inlineStr">
         <is>
           <t>Top &amp; right border</t>
         </is>
       </c>
-      <c r="C16" s="0"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="0" t="inlineStr">
+      <c r="A17" s="13" t="inlineStr">
         <is>
           <t>Dashed border</t>
         </is>
       </c>
-      <c r="B17" s="0" t="inlineStr">
+      <c r="B17" s="13" t="inlineStr">
         <is>
           <t>Dotted border</t>
         </is>
       </c>
-      <c r="C17" s="0" t="inlineStr">
+      <c r="C17" s="13" t="inlineStr">
         <is>
           <t>Double border</t>
         </is>
       </c>
-      <c r="D17" s="0"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="0" t="inlineStr">
+      <c r="A18" s="13" t="inlineStr">
         <is>
           <t>Solid border</t>
         </is>
       </c>
-      <c r="B18" s="0" t="inlineStr">
+      <c r="B18" s="13" t="inlineStr">
         <is>
           <t>Solid medium border</t>
         </is>
       </c>
-      <c r="C18" s="0" t="inlineStr">
+      <c r="C18" s="13" t="inlineStr">
         <is>
           <t>Solid thick border</t>
         </is>
       </c>
-      <c r="D18" s="0"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="0" t="inlineStr">
+      <c r="A19" s="7" t="inlineStr">
         <is>
           <t>Left align</t>
         </is>
       </c>
-      <c r="B19" s="0" t="inlineStr">
+      <c r="B19" s="19" t="inlineStr">
         <is>
           <t>Center align</t>
         </is>
       </c>
-      <c r="C19" s="0" t="inlineStr">
+      <c r="C19" s="20" t="inlineStr">
         <is>
           <t>Right align</t>
         </is>
       </c>
-      <c r="D19" s="0"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="0" t="inlineStr">
+      <c r="A20" s="9" t="inlineStr">
         <is>
           <t>Number format: currency</t>
         </is>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="21" t="n">
         <v>123456</v>
       </c>
-      <c r="C20" s="0"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="0" t="inlineStr">
+      <c r="A21" s="9" t="inlineStr">
         <is>
           <t>Number format: date</t>
         </is>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="22" t="n">
         <v>123456</v>
       </c>
-      <c r="C21" s="0"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="0" t="inlineStr">
+      <c r="A22" s="9" t="inlineStr">
         <is>
           <t>Number format: date_time</t>
         </is>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="23" t="n">
         <v>123456</v>
       </c>
-      <c r="C22" s="0"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23">
-      <c r="A23" s="0" t="inlineStr">
+      <c r="A23" s="9" t="inlineStr">
         <is>
           <t>Number format: number</t>
         </is>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="24" t="n">
         <v>123456</v>
       </c>
-      <c r="C23" s="0"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="0" t="inlineStr">
+      <c r="A24" s="9" t="inlineStr">
         <is>
           <t>Number format: percent</t>
         </is>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="25" t="n">
         <v>123456</v>
       </c>
-      <c r="C24" s="0"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25">
-      <c r="A25" s="0" t="inlineStr">
+      <c r="A25" s="9" t="inlineStr">
         <is>
           <t>Number format: text</t>
         </is>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="26" t="n">
         <v>123456</v>
       </c>
-      <c r="C25" s="0"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="0" t="inlineStr">
+      <c r="A26" s="9" t="inlineStr">
         <is>
           <t>Number format: time</t>
         </is>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="27" t="n">
         <v>123456</v>
       </c>
-      <c r="C26" s="0"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="0" t="inlineStr">
+      <c r="A27" s="9" t="inlineStr">
         <is>
           <t>Number format: scientific</t>
         </is>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="28" t="n">
         <v>123456</v>
       </c>
-      <c r="C27" s="0"/>
+      <c r="C27" s="9"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
excel border & number format support
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,6 +11,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <name val="Verdana"/>
@@ -75,8 +76,93 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="29">
     <border/>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="dashed"/>
+    </border>
+    <border>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+    </border>
+    <border>
+      <left style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+    </border>
+    <border>
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+    </border>
+    <border>
+      <top style="dotted"/>
+    </border>
+    <border>
+      <top style="dotted"/>
+      <bottom style="dotted"/>
+    </border>
+    <border>
+      <left style="dotted"/>
+      <top style="dotted"/>
+      <bottom style="dotted"/>
+    </border>
+    <border>
+      <left style="dotted"/>
+      <right style="dotted"/>
+      <top style="dotted"/>
+      <bottom style="dotted"/>
+    </border>
+    <border>
+      <top style="double"/>
+    </border>
+    <border>
+      <top style="double"/>
+      <bottom style="double"/>
+    </border>
+    <border>
+      <left style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
+    </border>
+    <border>
+      <left style="double"/>
+      <right style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
+    </border>
     <border>
       <top style="medium"/>
     </border>
@@ -96,23 +182,28 @@
       <bottom style="medium"/>
     </border>
     <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
+      <top style="thick"/>
+    </border>
+    <border>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,9 +256,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,13 +739,13 @@
       <c r="C16" s="0"/>
     </row>
     <row r="17" spans="1:4" customFormat="false">
-      <c r="A17" s="21" t="str">
+      <c r="A17" s="29" t="str">
         <v>Dashed border</v>
       </c>
-      <c r="B17" s="21" t="str">
+      <c r="B17" s="33" t="str">
         <v>Dotted border</v>
       </c>
-      <c r="C17" s="21" t="str">
+      <c r="C17" s="37" t="str">
         <v>Double border</v>
       </c>
       <c r="D17" s="0"/>
@@ -635,10 +754,10 @@
       <c r="A18" s="21" t="str">
         <v>Solid border</v>
       </c>
-      <c r="B18" s="21" t="str">
+      <c r="B18" s="41" t="str">
         <v>Solid medium border</v>
       </c>
-      <c r="C18" s="21" t="str">
+      <c r="C18" s="45" t="str">
         <v>Solid thick border</v>
       </c>
       <c r="D18" s="0"/>
@@ -650,7 +769,7 @@
       <c r="B19" s="2" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="26" t="str">
+      <c r="C19" s="46" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>
@@ -659,7 +778,7 @@
       <c r="A20" s="0" t="str">
         <v>Number format: currency</v>
       </c>
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="47" t="str">
         <v>123456</v>
       </c>
       <c r="C20" s="0"/>
@@ -668,7 +787,7 @@
       <c r="A21" s="0" t="str">
         <v>Number format: date</v>
       </c>
-      <c r="B21" s="0" t="str">
+      <c r="B21" s="48" t="str">
         <v>123456</v>
       </c>
       <c r="C21" s="0"/>
@@ -677,7 +796,7 @@
       <c r="A22" s="0" t="str">
         <v>Number format: date_time</v>
       </c>
-      <c r="B22" s="0" t="str">
+      <c r="B22" s="49" t="str">
         <v>123456</v>
       </c>
       <c r="C22" s="0"/>
@@ -686,7 +805,7 @@
       <c r="A23" s="0" t="str">
         <v>Number format: number</v>
       </c>
-      <c r="B23" s="0" t="str">
+      <c r="B23" s="50" t="str">
         <v>123456</v>
       </c>
       <c r="C23" s="0"/>
@@ -695,7 +814,7 @@
       <c r="A24" s="0" t="str">
         <v>Number format: percent</v>
       </c>
-      <c r="B24" s="0" t="str">
+      <c r="B24" s="51" t="str">
         <v>123456</v>
       </c>
       <c r="C24" s="0"/>
@@ -704,7 +823,7 @@
       <c r="A25" s="0" t="str">
         <v>Number format: text</v>
       </c>
-      <c r="B25" s="0" t="str">
+      <c r="B25" s="52" t="str">
         <v>123456</v>
       </c>
       <c r="C25" s="0"/>
@@ -713,7 +832,7 @@
       <c r="A26" s="0" t="str">
         <v>Number format: time</v>
       </c>
-      <c r="B26" s="0" t="str">
+      <c r="B26" s="53" t="str">
         <v>123456</v>
       </c>
       <c r="C26" s="0"/>
@@ -722,7 +841,7 @@
       <c r="A27" s="0" t="str">
         <v>Number format: scientific</v>
       </c>
-      <c r="B27" s="0" t="str">
+      <c r="B27" s="54" t="str">
         <v>123456</v>
       </c>
       <c r="C27" s="0"/>

</xml_diff>

<commit_message>
choose the first sheet if it's a new workbook
otherwise try to find the sheet by name or call add_worksheet
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Excel test" sheetId="2" r:id="rId4"/>
+    <sheet name="Excel test" sheetId="1" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -614,12 +613,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">

</xml_diff>

<commit_message>
extract a RubyXL-decorated Modifier
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -202,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +297,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +636,7 @@
       <c r="A1" s="3" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="4" t="str">
+      <c r="B1" s="55" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="8" t="str">
@@ -636,7 +653,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="56" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
make halign and valign distinctly different
trying to make them overlap and be smart about it just won't work. the
caller needs to be explicit
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,28 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -213,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,6 +323,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -633,19 +682,19 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="3" t="str">
+      <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="55" t="str">
+      <c r="B1" s="64" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="8" t="str">
+      <c r="C1" s="62" t="str">
         <v>Header3</v>
       </c>
       <c r="D1" s="11" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="3" t="str">
+      <c r="E1" s="57" t="str">
         <v>Header5</v>
       </c>
     </row>
@@ -653,7 +702,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="56" t="str">
+      <c r="B2" s="65" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">
@@ -776,7 +825,7 @@
       <c r="A19" s="12" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B19" s="1" t="str">
         <v>Center align</v>
       </c>
       <c r="C19" s="46" t="str">

</xml_diff>

<commit_message>
update changelog for v0.0.4, fix gemspec
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -235,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,6 +361,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -685,7 +702,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="64" t="str">
+      <c r="B1" s="66" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -702,7 +719,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="65" t="str">
+      <c r="B2" s="67" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
create bin/csvpp as an alias for csv++
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -246,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -367,6 +378,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -702,7 +719,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="66" t="str">
+      <c r="B1" s="68" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -719,7 +736,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="67" t="str">
+      <c r="B2" s="69" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
support for backing up before writes
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="20">
+  <fonts count="30">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,61 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -257,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +439,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -719,7 +804,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="68" t="str">
+      <c r="B1" s="78" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -736,7 +821,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="79" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
docs and test coverage
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="46">
+  <fonts count="52">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,39 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -400,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -605,6 +638,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -940,7 +991,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="94" t="str">
+      <c r="B1" s="100" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -957,7 +1008,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="95" t="str">
+      <c r="B2" s="101" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
extract benchmark logic into BenchmarkedCompiler
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="68">
+  <fonts count="76">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,50 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -521,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,6 +836,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1127,7 +1195,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="116" t="str">
+      <c r="B1" s="124" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1144,7 +1212,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="117" t="str">
+      <c r="B2" s="125" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
refactor Compiler.with_compiler to take a runtime
rather than taking the input/filename and constructing one
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="76">
+  <fonts count="82">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,39 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -565,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -860,6 +893,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1195,7 +1246,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="124" t="str">
+      <c r="B1" s="130" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1212,7 +1263,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="125" t="str">
+      <c r="B2" s="131" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
docs & test coverage
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="82">
+  <fonts count="94">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,72 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -598,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -911,6 +977,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1246,7 +1348,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="130" t="str">
+      <c r="B1" s="142" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1263,7 +1365,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="131" t="str">
+      <c r="B2" s="143" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
provide a bunch of builtins and revamp how they're called
* `cellnum`: The number (integer) of the current cell. Starts at 1

* `cellref`: A reference to the current cell

* `rowabove`: A reference to the row above

* `rowbelow`: A reference to the row below

* `rownum`: The number (integer) of the current row.  Starts at 1

* `rowref`: A reference to the current row

* `cellabove`: A reference to a cell above the current row

* `celladjacent`: A reference to a cell in the current row

* `cellbelow`: A reference to a cell below the current row
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="94">
+  <fonts count="98">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,28 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -664,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,6 +1035,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1348,7 +1382,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="142" t="str">
+      <c r="B1" s="146" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1365,7 +1399,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="143" t="str">
+      <c r="B2" s="147" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
verbose_summary for the compiled template
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="98">
+  <fonts count="108">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,61 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -686,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1047,6 +1102,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1382,7 +1467,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="146" t="str">
+      <c r="B1" s="156" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1399,7 +1484,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="147" t="str">
+      <c r="B2" s="157" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
use the ASTBuilder in the parsers
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="108">
+  <fonts count="110">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -741,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1132,6 +1143,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="107" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1467,7 +1484,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="156" t="str">
+      <c r="B1" s="158" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1484,7 +1501,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="157" t="str">
+      <c r="B2" s="159" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
better infix operator support
* add missing operators, handle %

* create a TOKEN_LIBRARY for reusability

* +Function+s now know if they're infix or not and preserve that.
  apparently excel doesn't support a bunch of the prefix functions we
  were converting to

* fix precedence
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="110">
+  <fonts count="116">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,39 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -752,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1149,6 +1182,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="109" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1484,7 +1535,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="158" t="str">
+      <c r="B1" s="164" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1501,7 +1552,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="159" t="str">
+      <c r="B2" s="165" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
fix bug with creating an excel sheet
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="116">
+  <fonts count="124">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,50 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -785,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1200,6 +1244,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="115" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1535,7 +1603,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="164" t="str">
+      <c r="B1" s="172" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1552,7 +1620,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="165" t="str">
+      <c r="B2" s="173" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
specs for google and rubyxl
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="124">
+  <fonts count="138">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,83 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -829,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1268,6 +1345,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="123" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1603,7 +1722,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="172" t="str">
+      <c r="B1" s="186" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1620,7 +1739,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="173" t="str">
+      <c r="B2" s="187" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
update README, split out some into docs/
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="138">
+  <fonts count="148">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,61 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -906,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1387,6 +1442,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="137" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1722,7 +1807,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="186" t="str">
+      <c r="B1" s="196" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1739,7 +1824,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="187" t="str">
+      <c r="B2" s="197" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
var= modifier which can bind variables to cells
To facilitate this I got rid of code_section and now Scope handles all
the binding of functions and variables.  Which is pretty much what you
would expect a scope to do
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="148">
+  <fonts count="150">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -961,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1472,6 +1483,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="147" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1807,7 +1824,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="196" t="str">
+      <c r="B1" s="198" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1824,7 +1841,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="197" t="str">
+      <c r="B2" s="199" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
this is officially a non-context free grammar
with the introduction of the var= feature, for better or worse I made
this now a non-context free grammar, which means the parser has hit it's
limits as far as parsing modifiers, so we're making it a little looser
and pushing some of it's logic into ValidatedModifier

- Create ValidatedModifier which decorates Modifier with all of the
  validation logic
- Better CLI handling of errors
- Improves the error hierarchy and adds a couple for parsing modifiers
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -972,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1490,6 +1490,24 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,30 +1839,30 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="57" t="str">
+      <c r="A1" s="200" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="198" t="str">
+      <c r="B1" s="200" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="62" t="str">
+      <c r="C1" s="202" t="str">
         <v>Header3</v>
       </c>
-      <c r="D1" s="11" t="str">
+      <c r="D1" s="203" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="57" t="str">
+      <c r="E1" s="200" t="str">
         <v>Header5</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="false">
-      <c r="A2" s="12" t="str">
+      <c r="A2" s="204" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="199" t="str">
+      <c r="B2" s="204" t="str">
         <v>=1</v>
       </c>
-      <c r="C2" s="12" t="str">
+      <c r="C2" s="204" t="str">
         <v>These are variables</v>
       </c>
       <c r="D2" s="0"/>
@@ -1961,13 +1979,13 @@
       <c r="D18" s="0"/>
     </row>
     <row r="19" spans="1:4" customFormat="false">
-      <c r="A19" s="12" t="str">
+      <c r="A19" s="204" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="1" t="str">
+      <c r="B19" s="200" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="46" t="str">
+      <c r="C19" s="205" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>

</xml_diff>

<commit_message>
move the parsers into one directory
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -972,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1490,6 +1490,24 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1839,30 +1857,30 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="200" t="str">
+      <c r="A1" s="206" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="200" t="str">
+      <c r="B1" s="206" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="202" t="str">
+      <c r="C1" s="208" t="str">
         <v>Header3</v>
       </c>
-      <c r="D1" s="203" t="str">
+      <c r="D1" s="209" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="200" t="str">
+      <c r="E1" s="206" t="str">
         <v>Header5</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="false">
-      <c r="A2" s="204" t="str">
+      <c r="A2" s="210" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="204" t="str">
+      <c r="B2" s="210" t="str">
         <v>=1</v>
       </c>
-      <c r="C2" s="204" t="str">
+      <c r="C2" s="210" t="str">
         <v>These are variables</v>
       </c>
       <c r="D2" s="0"/>
@@ -1979,13 +1997,13 @@
       <c r="D18" s="0"/>
     </row>
     <row r="19" spans="1:4" customFormat="false">
-      <c r="A19" s="204" t="str">
+      <c r="A19" s="210" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="200" t="str">
+      <c r="B19" s="206" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="205" t="str">
+      <c r="C19" s="211" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>

</xml_diff>

<commit_message>
get rid of language/ module
the whole thing is a language, it wasn't really conveying much meaning
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -972,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1490,6 +1490,24 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1857,30 +1875,30 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="206" t="str">
+      <c r="A1" s="212" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="206" t="str">
+      <c r="B1" s="212" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="208" t="str">
+      <c r="C1" s="214" t="str">
         <v>Header3</v>
       </c>
-      <c r="D1" s="209" t="str">
+      <c r="D1" s="215" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="206" t="str">
+      <c r="E1" s="212" t="str">
         <v>Header5</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="false">
-      <c r="A2" s="210" t="str">
+      <c r="A2" s="216" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="210" t="str">
+      <c r="B2" s="216" t="str">
         <v>=1</v>
       </c>
-      <c r="C2" s="210" t="str">
+      <c r="C2" s="216" t="str">
         <v>These are variables</v>
       </c>
       <c r="D2" s="0"/>
@@ -1997,13 +2015,13 @@
       <c r="D18" s="0"/>
     </row>
     <row r="19" spans="1:4" customFormat="false">
-      <c r="A19" s="210" t="str">
+      <c r="A19" s="216" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="206" t="str">
+      <c r="B19" s="212" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="211" t="str">
+      <c r="C19" s="217" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>

</xml_diff>

<commit_message>
richer support for parsing data validations
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -972,7 +972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1490,6 +1490,42 @@
     </xf>
     <xf numFmtId="0" fontId="149" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1875,30 +1911,30 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="212" t="str">
+      <c r="A1" s="224" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="212" t="str">
+      <c r="B1" s="224" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="214" t="str">
+      <c r="C1" s="226" t="str">
         <v>Header3</v>
       </c>
-      <c r="D1" s="215" t="str">
+      <c r="D1" s="227" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="212" t="str">
+      <c r="E1" s="224" t="str">
         <v>Header5</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="false">
-      <c r="A2" s="216" t="str">
+      <c r="A2" s="228" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="216" t="str">
+      <c r="B2" s="228" t="str">
         <v>=1</v>
       </c>
-      <c r="C2" s="216" t="str">
+      <c r="C2" s="228" t="str">
         <v>These are variables</v>
       </c>
       <c r="D2" s="0"/>
@@ -2015,13 +2051,13 @@
       <c r="D18" s="0"/>
     </row>
     <row r="19" spans="1:4" customFormat="false">
-      <c r="A19" s="216" t="str">
+      <c r="A19" s="228" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="212" t="str">
+      <c r="B19" s="224" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="217" t="str">
+      <c r="C19" s="229" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>

</xml_diff>

<commit_message>
refactor out a ::Modifier module
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="150">
+  <fonts count="152">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -972,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1580,6 +1591,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1911,30 +1928,30 @@
   <dimension ref="A1:E27"/>
   <sheetData>
     <row r="1" spans="1:5" customFormat="false">
-      <c r="A1" s="224" t="str">
+      <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="224" t="str">
+      <c r="B1" s="230" t="str">
         <v>Header2</v>
       </c>
-      <c r="C1" s="226" t="str">
+      <c r="C1" s="62" t="str">
         <v>Header3</v>
       </c>
-      <c r="D1" s="227" t="str">
+      <c r="D1" s="11" t="str">
         <v>Header4</v>
       </c>
-      <c r="E1" s="224" t="str">
+      <c r="E1" s="57" t="str">
         <v>Header5</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="false">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="228" t="str">
+      <c r="B2" s="231" t="str">
         <v>=1</v>
       </c>
-      <c r="C2" s="228" t="str">
+      <c r="C2" s="12" t="str">
         <v>These are variables</v>
       </c>
       <c r="D2" s="0"/>
@@ -2051,13 +2068,13 @@
       <c r="D18" s="0"/>
     </row>
     <row r="19" spans="1:4" customFormat="false">
-      <c r="A19" s="228" t="str">
+      <c r="A19" s="12" t="str">
         <v>Left align</v>
       </c>
-      <c r="B19" s="224" t="str">
+      <c r="B19" s="1" t="str">
         <v>Center align</v>
       </c>
-      <c r="C19" s="229" t="str">
+      <c r="C19" s="46" t="str">
         <v>Right align</v>
       </c>
       <c r="D19" s="0"/>

</xml_diff>

<commit_message>
remove Scope and include it's behavior into Runtime
no real need to have a scope that's separate from the runtime, and now
that the resolving variables depends on the runtime they pretty much
depend on each other enough that they might as well be the same thing.

but trying to preserve at least some separation of concerns by mixing in
the functionality
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="152">
+  <fonts count="154">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -983,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1596,6 +1607,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="151" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1931,7 +1948,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="230" t="str">
+      <c r="B1" s="232" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1948,7 +1965,7 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="231" t="str">
+      <c r="B2" s="233" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">

</xml_diff>

<commit_message>
a couple sorbet fixes
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="154">
+  <fonts count="158">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,28 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -994,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1613,6 +1635,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="153" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1948,7 +1982,7 @@
       <c r="A1" s="57" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="232" t="str">
+      <c r="B1" s="236" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="62" t="str">
@@ -1965,13 +1999,13 @@
       <c r="A2" s="12" t="str">
         <v>=ADD(1, 2)</v>
       </c>
-      <c r="B2" s="233" t="str">
+      <c r="B2" s="237" t="str">
         <v>=1</v>
       </c>
       <c r="C2" s="12" t="str">
         <v>These are variables</v>
       </c>
-      <c r="D2" s="0"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:2" customFormat="false">
       <c r="A3" s="0" t="str">

</xml_diff>

<commit_message>
runtime values are not entities
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="34">
+  <fonts count="38">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,28 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -334,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,6 +487,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,7 +828,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="76" t="str">
+      <c r="B1" s="80" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -816,7 +846,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="77">
+      <c r="B2" s="81">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
strict types for parsers and tokenizer
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="38">
+  <fonts count="52">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,83 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -356,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,6 +572,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,7 +933,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="80" t="str">
+      <c r="B1" s="94" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -846,7 +951,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="81">
+      <c r="B2" s="95">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
type coverage for variable resolution
this turned into a pretty big refactor which added:

* Runtime::Scope - just for storing and resolving function and variale
  references

* Runtime::Position - stores all the line_number/cell_index/row_index
  counters and functions for tracking/mapping them

* ErrorFormatter - combines an Options and Position to format an error
  message

  *

and:

* add types to the Racc parsers

* refactored and added types to the Error:: classes

* types for the lexers and tokenizer
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="52">
+  <fonts count="54">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -433,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,6 +611,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,7 +948,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="94" t="str">
+      <c r="B1" s="96" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -951,7 +966,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="95">
+      <c r="B2" s="97">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
strict types for FileBackerUpper
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="54">
+  <fonts count="56">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -444,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,6 +626,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,7 +963,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="96" t="str">
+      <c r="B1" s="98" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -966,7 +981,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="97">
+      <c r="B2" s="99">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
get rid of variable dereference operator ($$)
instead we make the CellReference into a more general Reference which is
able to either act like it's previous self, or just a ref to a variable.
And now we only interpolate variables if they are defined, otherwise
just leave it alone
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="56">
+  <fonts count="68">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,72 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -455,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -630,6 +696,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,7 +1053,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="98" t="str">
+      <c r="B1" s="110" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -981,7 +1071,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="99">
+      <c r="B2" s="111">
         <f>1</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
use the output_filename if sheet_name is not given
</commit_message>
<xml_diff>
--- a/examples/all_features.xlsx
+++ b/examples/all_features.xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
   <numFmts count="0"/>
-  <fonts count="68">
+  <fonts count="70">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -60,6 +60,17 @@
     <font>
       <name val="Verdana"/>
       <sz val="20"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <sz val="10"/>
+      <u val="1"/>
     </font>
     <font>
       <name val="Verdana"/>
@@ -521,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -720,6 +731,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1068,7 @@
       <c r="A1" s="2" t="str">
         <v>Header1</v>
       </c>
-      <c r="B1" s="110" t="str">
+      <c r="B1" s="112" t="str">
         <v>Header2</v>
       </c>
       <c r="C1" s="7" t="str">
@@ -1071,7 +1086,7 @@
         <f>(1 + 2)</f>
         <v/>
       </c>
-      <c r="B2" s="111">
+      <c r="B2" s="113">
         <f>1</f>
         <v/>
       </c>

</xml_diff>